<commit_message>
mandatory heating technology modernization added
</commit_message>
<xml_diff>
--- a/projects/test_building/input/ID_EnergyCarrier.xlsx
+++ b/projects/test_building/input/ID_EnergyCarrier.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F677712-5574-5A4B-B4A2-269751F70840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62CE861B-94B3-3D49-8468-CD08697BD2A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28740" yWindow="-21100" windowWidth="23320" windowHeight="19400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -454,12 +454,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="191" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>